<commit_message>
end of day - more tests added
</commit_message>
<xml_diff>
--- a/gradingChecklist.xlsx
+++ b/gradingChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/ComputerScienceBSc/DataStructuresAndAlgorithms1/intellijProjects/JS1/JS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="8_{CAC91B45-3C00-4E6B-ABF0-F5400BF4DE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBC6AA94-EE92-49DF-85B7-B2AAA83CA6A8}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="8_{CAC91B45-3C00-4E6B-ABF0-F5400BF4DE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05AFD612-639B-4D79-9A78-A2CABF229504}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="225" windowWidth="14385" windowHeight="14745" xr2:uid="{21DF9608-6AA7-46E1-9B20-46CB7C238BD0}"/>
+    <workbookView xWindow="14100" yWindow="540" windowWidth="14385" windowHeight="14745" xr2:uid="{21DF9608-6AA7-46E1-9B20-46CB7C238BD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
   <si>
     <t>ID#</t>
   </si>
   <si>
-    <t>Yes/No</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -230,18 +227,12 @@
     <t>Interactive view stock  /           Drill down</t>
   </si>
   <si>
-    <t>clickable view all ?</t>
-  </si>
-  <si>
     <t>Jewellery Material</t>
   </si>
   <si>
     <t>Reset (Delete) all stock</t>
   </si>
   <si>
-    <t>Marked out of --&gt;&gt;</t>
-  </si>
-  <si>
     <t>Create Sample Stock Data</t>
   </si>
   <si>
@@ -251,9 +242,6 @@
     <t>Value Stock - All Case &amp; Trays &amp; Items &amp; Materials</t>
   </si>
   <si>
-    <t>8 - 10 tests</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
@@ -264,6 +252,39 @@
   </si>
   <si>
     <t>Attempted?</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>clickable to expand</t>
+  </si>
+  <si>
+    <t>Add on - clock</t>
+  </si>
+  <si>
+    <t>Add on - countdown timer</t>
+  </si>
+  <si>
+    <t>countdown to Christmas!</t>
+  </si>
+  <si>
+    <t>a bit of fun.</t>
+  </si>
+  <si>
+    <t>Add on - clickable pic with reveal</t>
+  </si>
+  <si>
+    <t>custom linked lists</t>
+  </si>
+  <si>
+    <t>Possible %</t>
+  </si>
+  <si>
+    <t>Edit Jewellery item</t>
+  </si>
+  <si>
+    <t>Delete Jewellery item</t>
   </si>
 </sst>
 </file>
@@ -375,6 +396,10 @@
     </a>
   </bag>
 </FeaturePropertyBags>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F0309E-2FAD-41F1-809D-AC724CA6B96D}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,33 +734,36 @@
     <col min="5" max="5" width="11.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="35.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="34.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="29.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="11" max="11" width="11" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="L1" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -746,25 +774,28 @@
         <v>123</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="H2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="K2" s="6">
         <v>0.1</v>
@@ -772,38 +803,35 @@
       <c r="L2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="6">
-        <f>IF(L2,K2,0)</f>
-        <v>0.1</v>
-      </c>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="6">
         <v>0.12</v>
@@ -811,41 +839,38 @@
       <c r="L3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M3" s="6">
-        <f t="shared" ref="M3:M14" si="0">IF(L3,K3,0)</f>
-        <v>0.12</v>
-      </c>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="H4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4" s="6">
         <v>0.08</v>
@@ -853,26 +878,23 @@
       <c r="L4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M4" s="6">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="H5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="K5" s="6">
         <v>7.0000000000000007E-2</v>
@@ -880,26 +902,23 @@
       <c r="L5" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="6">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H6" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K6" s="6">
         <v>0.1</v>
@@ -907,32 +926,29 @@
       <c r="L6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M6" s="6">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="6">
         <v>0.1</v>
@@ -940,32 +956,29 @@
       <c r="L7" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M7" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E8" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="6">
         <v>0.05</v>
@@ -973,32 +986,29 @@
       <c r="L8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M8" s="6">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H9" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K9" s="6">
         <v>0.1</v>
@@ -1006,32 +1016,29 @@
       <c r="L9" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M9" s="6">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H10" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K10" s="6">
         <v>0.05</v>
@@ -1039,20 +1046,17 @@
       <c r="L10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M10" s="6">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" s="6">
         <v>0.08</v>
@@ -1060,23 +1064,20 @@
       <c r="L11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M11" s="6">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" s="6">
         <v>0.05</v>
@@ -1084,59 +1085,59 @@
       <c r="L12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M12" s="6">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K13" s="6">
         <v>0.05</v>
       </c>
       <c r="L13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="F14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="I14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14" s="6">
         <v>0.05</v>
@@ -1144,51 +1145,49 @@
       <c r="L14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M14" s="6">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="F15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="6">
-        <f>SUM(M2:M14)</f>
-        <v>0.85000000000000009</v>
-      </c>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E16" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="5" t="b">
         <v>1</v>
@@ -1196,22 +1195,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E17" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H17" s="5" t="b">
         <v>1</v>
@@ -1219,22 +1218,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" s="5" t="b">
         <v>1</v>
@@ -1242,22 +1241,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H19" s="5" t="b">
         <v>1</v>
@@ -1265,18 +1264,18 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
       <c r="H20" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="H21" s="5" t="b">
         <v>0</v>
@@ -1290,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="H22" s="5" t="b">
         <v>0</v>
@@ -1298,33 +1297,39 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>48</v>
+        <v>75</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="H23" s="5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="H24" s="5" t="b">
         <v>0</v>
@@ -1332,19 +1337,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="H25" s="5" t="b">
         <v>0</v>
@@ -1352,22 +1354,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E26" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="H26" s="5" t="b">
         <v>0</v>
@@ -1375,13 +1374,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="5" t="b">
         <v>1</v>
@@ -1389,19 +1388,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H28" s="5" t="b">
         <v>1</v>
@@ -1409,13 +1408,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="5" t="b">
         <v>1</v>
@@ -1423,7 +1422,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F30" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H30" s="5" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Style and layout updates. Remove redundant/default tags & unwrap children, etc.
</commit_message>
<xml_diff>
--- a/gradingChecklist.xlsx
+++ b/gradingChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f35c4a080af5b301/Documents/ComputerScienceBSc/DataStructuresAndAlgorithms1/intellijProjects/JS1/JS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="8_{CAC91B45-3C00-4E6B-ABF0-F5400BF4DE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05AFD612-639B-4D79-9A78-A2CABF229504}"/>
+  <xr:revisionPtr revIDLastSave="381" documentId="8_{CAC91B45-3C00-4E6B-ABF0-F5400BF4DE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{143BC1AE-3307-4B0A-B52E-2073945DE462}"/>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="540" windowWidth="14385" windowHeight="14745" xr2:uid="{21DF9608-6AA7-46E1-9B20-46CB7C238BD0}"/>
+    <workbookView xWindow="1290" yWindow="540" windowWidth="27195" windowHeight="14745" xr2:uid="{21DF9608-6AA7-46E1-9B20-46CB7C238BD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>ID#</t>
   </si>
@@ -285,6 +285,30 @@
   </si>
   <si>
     <t>Delete Jewellery item</t>
+  </si>
+  <si>
+    <t>TO DO:</t>
+  </si>
+  <si>
+    <t>Allow user to specify filename to load/save data.</t>
+  </si>
+  <si>
+    <t>with backup(s)</t>
+  </si>
+  <si>
+    <t>clear lists</t>
+  </si>
+  <si>
+    <t>Total value . Also by cases, trays, items, + materials.</t>
+  </si>
+  <si>
+    <t>not yet…</t>
+  </si>
+  <si>
+    <t>Smart search</t>
+  </si>
+  <si>
+    <t>need to redesign cases &amp; trays to set item number and size limits. Should have done this at the beginning!</t>
   </si>
 </sst>
 </file>
@@ -721,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F0309E-2FAD-41F1-809D-AC724CA6B96D}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,6 +974,9 @@
       <c r="I7" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="K7" s="6">
         <v>0.1</v>
       </c>
@@ -1010,6 +1037,9 @@
       <c r="I9" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="J9" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="K9" s="6">
         <v>0.1</v>
       </c>
@@ -1040,6 +1070,9 @@
       <c r="I10" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="J10" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="K10" s="6">
         <v>0.05</v>
       </c>
@@ -1058,6 +1091,9 @@
       <c r="I11" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="K11" s="6">
         <v>0.08</v>
       </c>
@@ -1193,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1216,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1238,8 +1274,11 @@
       <c r="H18" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1261,8 +1300,11 @@
       <c r="H19" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
         <v>47</v>
       </c>
@@ -1273,15 +1315,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1292,10 +1337,10 @@
         <v>74</v>
       </c>
       <c r="H22" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>11</v>
       </c>
@@ -1312,10 +1357,10 @@
         <v>76</v>
       </c>
       <c r="H23" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
@@ -1332,10 +1377,10 @@
         <v>77</v>
       </c>
       <c r="H24" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1348,11 +1393,8 @@
       <c r="E25" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H25" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1368,11 +1410,8 @@
       <c r="E26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
@@ -1386,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -1399,14 +1438,8 @@
       <c r="E28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -1419,9 +1452,15 @@
       <c r="E29" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="4" t="s">
+      <c r="F29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H30" s="5" t="b">

</xml_diff>